<commit_message>
reorder linkedlist optimal solution
</commit_message>
<xml_diff>
--- a/AlgoSheet/Algosheet.xlsx
+++ b/AlgoSheet/Algosheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/AlgoSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9349056-AC9C-1D41-BBA4-5DD15E8B3894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A605D3-E199-784C-8B94-51E0323E282C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27680" yWindow="2360" windowWidth="23360" windowHeight="14660" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="73">
   <si>
     <t>Category</t>
   </si>
@@ -408,6 +408,78 @@
   </si>
   <si>
     <t>Merge Two Sorted Lists </t>
+  </si>
+  <si>
+    <t>Linked List Cycle </t>
+  </si>
+  <si>
+    <t>Store nodes in hashmap and keep checking, if you find a cycle the nodes would repeat. 
+initialize temp to head and dictionary d to empty
+while temp is not None:
+    if temp in d:
+        return True
+    add temp to d
+    move temp to temp.next
+return False</t>
+  </si>
+  <si>
+    <t>just read code. If you insist:
+initialize slow and fast to head
+while fast and fast.next:
+    move slow one step forward
+    if fast.next:
+        move fast two steps forward
+    else:
+        return False #fast has reached the end, so if won't move anymore, end it here
+    if slow equals fast:
+        return True
+return False</t>
+  </si>
+  <si>
+    <t>two pointers , one slow and one fast. If there's a cycle, slow will eventually catch up to fast. Kind of like how in circuit races, one car might just overlap the other, and actually be multiple laps ahead technically because it was too fast</t>
+  </si>
+  <si>
+    <t>Reorder List </t>
+  </si>
+  <si>
+    <t>Just store the nodes in a deque and manipulate accordingly.
+initialize deque d
+set temp to head
+while temp is not None:
+    add temp to d
+    move temp to temp.next
+while d is not empty:
+    if temp is None:
+        set temp to d.popleft()
+    else:
+        set temp.next to d.popleft()
+        move temp to temp.next
+    if d is not empty:
+        set temp.next to d.pop()
+        move temp to temp.next
+set temp.next to None</t>
+  </si>
+  <si>
+    <t>same as Merge Two sorted lists. Find halfway node of the linked list using fast and slow pointers, consider them as two separate linked lists. Reverse the second one because we want to traverse from the end and then merge them(instead of comparing their values just alternate between the two</t>
+  </si>
+  <si>
+    <t>Find the middle of the list:-
+Initialize slow and fast pointers at the head.
+Move slow by one step and fast by two steps until fast or fast.next is null.
+Reverse the second half of the list:-
+Initialize second as slow.next and prev as null.
+Set slow.next to null to split the list.
+While second is not null:
+Store second.next in a temporary variable tmp.
+Set second.next to prev.
+Move prev and second one step forward.
+Merge the two halves:-
+Initialize first as head and second as prev.
+While second is not null:
+Store first.next and second.next in tmp1 and tmp2.
+Set first.next to second.
+Set second.next to tmp1.
+Move first and second one step forward.</t>
   </si>
 </sst>
 </file>
@@ -837,8 +909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D8D0A7-2B23-DB41-A123-92CA1A1D8EFD}">
   <dimension ref="A1:S216"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1176,12 +1248,48 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="F14" t="s">
         <v>13</v>
       </c>
+      <c r="G14" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1696,6 +1804,8 @@
     <hyperlink ref="B11" r:id="rId10" display="https://neetcode.io/problems/find-target-in-rotated-sorted-array" xr:uid="{510497A1-3ACB-1A40-A017-2B211237C3EC}"/>
     <hyperlink ref="B12" r:id="rId11" display="https://neetcode.io/problems/reverse-a-linked-list" xr:uid="{F1D5B347-75DA-8F44-95F4-EBC12A45E144}"/>
     <hyperlink ref="B13" r:id="rId12" display="https://neetcode.io/problems/merge-two-sorted-linked-lists" xr:uid="{00F47F2F-ECD3-3D47-AE36-BB55D6CA3DE2}"/>
+    <hyperlink ref="B14" r:id="rId13" display="https://neetcode.io/problems/linked-list-cycle-detection" xr:uid="{C73BD96A-E0F9-074A-8348-9F342D5C5307}"/>
+    <hyperlink ref="B15" r:id="rId14" display="https://neetcode.io/problems/reorder-linked-list" xr:uid="{AA53E998-81B8-834C-923C-9B76814166B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
remove nth node from end
</commit_message>
<xml_diff>
--- a/AlgoSheet/Algosheet.xlsx
+++ b/AlgoSheet/Algosheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/AlgoSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A605D3-E199-784C-8B94-51E0323E282C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D31E0A64-1BF2-2646-B106-925DE0964AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27680" yWindow="2360" windowWidth="23360" windowHeight="14660" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="77">
   <si>
     <t>Category</t>
   </si>
@@ -480,6 +480,24 @@
 Set first.next to second.
 Set second.next to tmp1.
 Move first and second one step forward.</t>
+  </si>
+  <si>
+    <t>Remove Nth Node From End of List </t>
+  </si>
+  <si>
+    <t>traverse through linkedlist twice . First to find which number is at the index from the end. Traverse again to delete</t>
+  </si>
+  <si>
+    <t>two pointers, first move fast pointer by  n places, then traverse once to find and delete at slow pointer</t>
+  </si>
+  <si>
+    <t>1. Create a dummy node pointing to the head
+2. Initialize left and right pointers at dummy and head
+3. Move right pointer n steps forward
+4. While right is not null:
+   a. Move left and right pointers one step forward
+5. Set left.next to left.next.next to remove the nth node from end
+6. Return dummy.next as the new head of the list</t>
   </si>
 </sst>
 </file>
@@ -909,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D8D0A7-2B23-DB41-A123-92CA1A1D8EFD}">
   <dimension ref="A1:S216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1294,7 +1312,25 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>74</v>
+      </c>
       <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1806,6 +1842,7 @@
     <hyperlink ref="B13" r:id="rId12" display="https://neetcode.io/problems/merge-two-sorted-linked-lists" xr:uid="{00F47F2F-ECD3-3D47-AE36-BB55D6CA3DE2}"/>
     <hyperlink ref="B14" r:id="rId13" display="https://neetcode.io/problems/linked-list-cycle-detection" xr:uid="{C73BD96A-E0F9-074A-8348-9F342D5C5307}"/>
     <hyperlink ref="B15" r:id="rId14" display="https://neetcode.io/problems/reorder-linked-list" xr:uid="{AA53E998-81B8-834C-923C-9B76814166B7}"/>
+    <hyperlink ref="B16" r:id="rId15" display="https://neetcode.io/problems/remove-node-from-end-of-linked-list" xr:uid="{3978F454-A1ED-2E47-B297-93196592774C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
bucket sort+top k freq
</commit_message>
<xml_diff>
--- a/AlgoSheet/Algosheet.xlsx
+++ b/AlgoSheet/Algosheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/AlgoSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7754E76D-182A-794E-9C77-E9A4BCC7FAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97458717-99B3-E74D-932C-05805D2BA542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27680" yWindow="2360" windowWidth="23360" windowHeight="14660" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="109">
   <si>
     <t>Category</t>
   </si>
@@ -636,12 +636,151 @@
   <si>
     <t xml:space="preserve"> code finds if a word exists in a grid by exploring all possible paths starting from each cell. It uses a helper function to recursively check each letter of the word, moving up, down, left, or right, while avoiding revisiting cells. It optimizes by reversing the word if needed to reduce search time. The function returns true if the word is found, otherwise false.</t>
   </si>
+  <si>
+    <t>optimal 1:
+class Solution:
+    def containsDuplicate(self, nums: List[int]) -&gt; bool:
+        return len(set(nums))!=len(nums)</t>
+  </si>
+  <si>
+    <t>optimal 2:
+class Solution:
+    def containsDuplicate(self, nums: List[int]) -&gt; bool:
+        hashset = set()
+        for n in nums:
+            if n in hashset:
+                return True
+            hashset.add(n)
+        return False</t>
+  </si>
+  <si>
+    <t>store in hashmap and check. Alternate is set() and len() approach</t>
+  </si>
+  <si>
+    <t>Arrays &amp; Hashing</t>
+  </si>
+  <si>
+    <t>Contains Duplicate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">from collections import Counter
+class Solution:
+    def isAnagram(self, s: str, t: str) -&gt; bool:
+        return Counter(s)==Counter(t)
+        </t>
+  </si>
+  <si>
+    <t>Count frequency of each character store in hashmap and compare</t>
+  </si>
+  <si>
+    <t>Valid Anagram </t>
+  </si>
+  <si>
+    <t>class Solution:
+    def twoSum(self, nums: List[int], target: int) -&gt; List[int]:
+        h={}
+        for i in range(len(nums)):
+            key=target-nums[i]
+            if key in h:
+                return [h[key],i]
+            h[nums[i]]=i</t>
+  </si>
+  <si>
+    <t>as you iterate, store value and index in hash. Start of every iteration check if current number is in hashmap. If so, return those indices</t>
+  </si>
+  <si>
+    <t>Two Sum </t>
+  </si>
+  <si>
+    <t>Group Anagrams </t>
+  </si>
+  <si>
+    <t>class Solution:
+    def groupAnagrams(self, strs: List[str]) -&gt; List[List[str]]:
+        ans = collections.defaultdict(list)
+        for s in strs:
+            count = [0] * 26
+            for c in s:
+                count[ord(c) - ord("a")] += 1
+            ans[tuple(count)].append(s)
+        return ans.values()</t>
+  </si>
+  <si>
+    <t>see optimal solution, more interesting and only slightly complex than brute force</t>
+  </si>
+  <si>
+    <t>class Solution:
+    def groupAnagrams(self, strs: List[str]) -&gt; List[List[str]]:
+        d={}
+        for s in strs:
+            temp=str(sorted(list(s)))
+            if temp in d:
+                d[temp].append(s)
+            else:
+                d[temp]=[s]
+        return list(d.values())
+- **brute soln**: Time: \(O(N K \log K)\), Space: \(O(N K)\)
+- **optimal soln**: Time: \(O(N K)\), Space: \(O(N K)\)</t>
+  </si>
+  <si>
+    <t>Top K Frequent Elements </t>
+  </si>
+  <si>
+    <t>to do it in O(n) time instead of O(nlogn) that we need to sort it</t>
+  </si>
+  <si>
+    <t>optimal (second most efficient. compared to bucket sort solution)
+class Solution:
+    def topKFrequent(self, nums: List[int], k: int) -&gt; List[int]:
+        d=Counter(nums) #count frequency of elements
+        heapmax=[[-freq,num] for num,freq in d.items()] #heapq has only min heap so treating numbers as negative will make it act as a max heap
+        heapq.heapify(heapmax) #heapify creates heap. take O(n) time
+        list1=[] #to store k most freq elements
+        for i in range(k):
+            poping=heapq.heappop(heapmax) #extract max element
+            list1.append(poping[1]) #append value into the list
+        return list1
+brute force:
+from collections import Counter
+from collections import OrderedDict
+class Solution:
+    def topKFrequent(self, nums: List[int], k: int) -&gt; List[int]:
+        d = Counter(nums) 
+        d = OrderedDict(reversed(sorted(d.items(), key=lambda item: item[1])))
+        return list(d.keys())[:k]
+- **Code 1**: Time: \(O(N)\), Space: \(O(N)\)
+- **Code 2**: Time: \(O(N \log N)\), Space: \(O(N)\)
+Code 1 is more efficient in both time and space complexity.</t>
+  </si>
+  <si>
+    <t>most optimal is using bucket sort, second best optimal one is using max heap(which is written under brute force column of this row)
+code:
+class Solution:
+    method topKFrequent(nums, k):
+        initialize count as empty dictionary
+        initialize freq as list of empty lists with size len(nums) + 1
+        for each n in nums:
+            count[n] = 1 + count.get(n, 0)
+        for each (n, c) in count.items():
+            append n to freq[c]
+        initialize res as empty list
+        for i from len(freq) - 1 to 1 (inclusive):
+            for each n in freq[i]:
+                append n to res
+                if length of res equals k:
+                    return res
+Sure! Imagine you have a box of colored balls, and you want to find the k colors that appear the most often. Here's how you can think about the solution:
+1. **Counting Colors**: First, we go through all the balls and count how many there are of each color. It's like making a list of each color and noting down how many balls of that color you have.
+2. **Organizing by Frequency**: Next, we take this list and sort the colors into groups based on how many balls of each color there are. For example, we might have a group for colors that appear 3 times, another group for colors that appear 5 times, and so on.
+3. **Finding the Most Frequent Colors**: Finally, we look at the groups starting from the one with the most balls and pick the colors from those groups until we've found the k most frequent ones. It's like picking the most popular colors until you have the number you need.
+By organizing and counting the balls in this way, we can quickly find the most frequent colors without having to repeatedly compare every single ball to every other one.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -677,6 +816,14 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -705,7 +852,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -727,6 +874,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1064,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D8D0A7-2B23-DB41-A123-92CA1A1D8EFD}">
   <dimension ref="A1:S216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1541,27 +1699,111 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="F20" t="s">
         <v>13</v>
       </c>
+      <c r="G20" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>95</v>
+      </c>
       <c r="F21" t="s">
         <v>13</v>
       </c>
+      <c r="G21" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="F22" t="s">
         <v>13</v>
       </c>
+      <c r="G22" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>104</v>
+      </c>
       <c r="F23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F24" t="s">
+      <c r="G23" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2037,6 +2279,11 @@
     <hyperlink ref="B17" r:id="rId16" display="https://neetcode.io/problems/merge-k-sorted-linked-lists" xr:uid="{9C3CE5D7-5815-8B46-A597-056735108E1F}"/>
     <hyperlink ref="B18" r:id="rId17" display="https://neetcode.io/problems/combination-target-sum" xr:uid="{D707242E-14DF-5D4E-AFFE-C84916685B71}"/>
     <hyperlink ref="B19" r:id="rId18" display="https://neetcode.io/problems/search-for-word" xr:uid="{BF516528-D0FF-A643-A8D9-B94190B50B3C}"/>
+    <hyperlink ref="B20" r:id="rId19" display="https://neetcode.io/problems/duplicate-integer" xr:uid="{3875B682-ED40-3242-9FA6-D90119162AF7}"/>
+    <hyperlink ref="B21" r:id="rId20" display="https://neetcode.io/problems/is-anagram" xr:uid="{2B57C655-1386-C947-858F-4317FDFB0D92}"/>
+    <hyperlink ref="B22" r:id="rId21" display="https://neetcode.io/problems/two-integer-sum" xr:uid="{527061F0-9AAF-1A40-A47D-95537613298E}"/>
+    <hyperlink ref="B23" r:id="rId22" display="https://neetcode.io/problems/anagram-groups" xr:uid="{70FC1425-DCD0-9543-BF04-BD7D6821FAF1}"/>
+    <hyperlink ref="B24" r:id="rId23" display="https://neetcode.io/problems/top-k-elements-in-list" xr:uid="{E953D456-BAC4-2F43-9A19-DF33BD3496C6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
arrays longest consecutive seq+product except self
</commit_message>
<xml_diff>
--- a/AlgoSheet/Algosheet.xlsx
+++ b/AlgoSheet/Algosheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/AlgoSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97458717-99B3-E74D-932C-05805D2BA542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0109EBBB-0830-D148-8A69-9F6CA63F14F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27680" yWindow="2360" windowWidth="23360" windowHeight="14660" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="117">
   <si>
     <t>Category</t>
   </si>
@@ -774,6 +774,76 @@
 2. **Organizing by Frequency**: Next, we take this list and sort the colors into groups based on how many balls of each color there are. For example, we might have a group for colors that appear 3 times, another group for colors that appear 5 times, and so on.
 3. **Finding the Most Frequent Colors**: Finally, we look at the groups starting from the one with the most balls and pick the colors from those groups until we've found the k most frequent ones. It's like picking the most popular colors until you have the number you need.
 By organizing and counting the balls in this way, we can quickly find the most frequent colors without having to repeatedly compare every single ball to every other one.</t>
+  </si>
+  <si>
+    <t>function productExceptSelf(nums):
+    initialize res as an array of ones with length of nums
+    # Calculate prefix products
+    for i from 1 to length of nums - 1:
+        res[i] = res[i-1] * nums[i-1]
+    initialize postfix as 1
+    # Calculate postfix products and final result
+    for i from length of nums - 1 to 0:
+        res[i] *= postfix
+        postfix *= nums[i]
+    return res</t>
+  </si>
+  <si>
+    <t>second most optimal solution:
+function productExceptSelf(nums):
+    initialize res as an array of ones with length of nums
+    initialize prefix as an empty array
+    initialize preprod as 1
+    # Calculate prefix products
+    for each element in nums:
+        preprod *= element
+        append preprod to prefix
+    initialize suffix as an empty array
+    initialize sufprod as 1
+    # Calculate suffix products
+    for each element in nums, reversed:
+        sufprod *= element
+        insert sufprod at the beginning of suffix
+    initialize result as an empty array
+    # Calculate the product of elements except self
+    for i from 0 to length of nums - 1:
+        if i &gt; 0:
+            pre = prefix[i-1]
+        else:
+            pre = 1
+        if i &lt; length of nums - 1:
+            suf = suffix[i+1]
+        else:
+            suf = 1
+        append pre * suf to result
+    return result</t>
+  </si>
+  <si>
+    <t>Imagine you have a list of numbers and want to create a new list where each position contains the product of all the original numbers except the one at that position. We first multiply numbers to the left, then to the right of each position, without including the number at that position itself. This way, everyone gets the total without counting themselves.</t>
+  </si>
+  <si>
+    <t>Product of Array Except Self </t>
+  </si>
+  <si>
+    <t>function longestConsecutive(nums):
+    convert nums to a set called numSet
+    initialize longest to 0
+    for each n in numSet:
+        if (n - 1) is not in numSet:  # Check if n is the start of a sequence
+            initialize length to 1
+            while (n + length) is in numSet:
+                increment length by 1
+            longest = max(longest, length)
+    return longest</t>
+  </si>
+  <si>
+    <t>Longest Consecutive Sequence </t>
+  </si>
+  <si>
+    <t>To find the longest streak of consecutive numbers in a list, we first put all the numbers into a set for easy checking. Then, for each number, we see if it's the start of a new streak by checking if there's no number before it. If it is, we count how long the streak goes by checking consecutive numbers. We keep track of the longest streak found.</t>
+  </si>
+  <si>
+    <t>brute force would have been to sort it. Which the problem discourages</t>
   </si>
 </sst>
 </file>
@@ -852,7 +922,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -874,17 +944,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1223,7 +1283,7 @@
   <dimension ref="A1:S216"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23:G24"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1784,23 +1844,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="11" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+    <row r="24" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>93</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F24" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="4" t="s">
@@ -1808,12 +1868,48 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="F25" t="s">
         <v>13</v>
       </c>
+      <c r="G25" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>93</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>116</v>
+      </c>
       <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2284,6 +2380,8 @@
     <hyperlink ref="B22" r:id="rId21" display="https://neetcode.io/problems/two-integer-sum" xr:uid="{527061F0-9AAF-1A40-A47D-95537613298E}"/>
     <hyperlink ref="B23" r:id="rId22" display="https://neetcode.io/problems/anagram-groups" xr:uid="{70FC1425-DCD0-9543-BF04-BD7D6821FAF1}"/>
     <hyperlink ref="B24" r:id="rId23" display="https://neetcode.io/problems/top-k-elements-in-list" xr:uid="{E953D456-BAC4-2F43-9A19-DF33BD3496C6}"/>
+    <hyperlink ref="B25" r:id="rId24" display="https://neetcode.io/problems/products-of-array-discluding-self" xr:uid="{CE7DC939-4F90-A44D-9EF1-2DF54DACEE71}"/>
+    <hyperlink ref="B26" r:id="rId25" display="https://neetcode.io/problems/longest-consecutive-sequence" xr:uid="{4E062C1B-ADA0-3843-82F2-8C669E1F440E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
k smallest element in bst
</commit_message>
<xml_diff>
--- a/AlgoSheet/Algosheet.xlsx
+++ b/AlgoSheet/Algosheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/AlgoSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4412E90E-9AE5-424E-B2CC-A07830D748AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAAAAE0-FC4D-454C-AEE8-144BDA2CE4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27680" yWindow="2360" windowWidth="23360" windowHeight="14660" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="159">
   <si>
     <t>Category</t>
   </si>
@@ -1163,6 +1163,90 @@
   <si>
     <t>just see second-most optimal solution code:
 visiting each level of a tree one by one and recording the values of the nodes at each level. It uses a method to go through the tree from top to bottom, keeping track of which level each node is on. The final output is a list of lists, where each inner list contains the values of the nodes at that level of the tree.</t>
+  </si>
+  <si>
+    <t># Definition for a binary tree node.
+# class TreeNode:
+#     def __init__(self, val=0, left=None, right=None):
+#         self.val = val
+#         self.left = left
+#         self.right = right
+class Solution:
+    def isValidBST(self, root: TreeNode) -&gt; bool:
+        def valid(node, left, right):
+            if not node:
+                return True
+            if not (left &lt; node.val &lt; right):
+                return False
+            return valid(node.left, left, node.val) and valid(
+                node.right, node.val, right
+            )
+        return valid(root, float("-inf"), float("inf"))</t>
+  </si>
+  <si>
+    <t>The code checks if a binary tree is a valid binary search tree (BST). A BST is a tree where each node has at most two children, and for every node, all values in its left subtree are smaller, and all values in its right subtree are larger. The function starts at the root and verifies these rules recursively for every node. It uses minimum and maximum bounds to ensure each node's value is within the valid range. If all nodes follow the BST rules, the tree is considered valid.</t>
+  </si>
+  <si>
+    <t>brute force(works for any treee:
+# Definition for a binary tree node.
+# class TreeNode:
+#     def __init__(self, val=0, left=None, right=None):
+#         self.val = val
+#         self.left = left
+#         self.right = right
+#use maxheap, compare root and if value&lt;root, pop root and push this value in
+#return root after traversal is done
+import heapq
+class Solution:
+    def __init__(self):
+        self.smallnums=[] #empty minheap, but we need maxheap, so we insert negatives
+    def traverse(self, root, k):
+        if root:
+            self.traverse(root.left, k)
+            if len(self.smallnums)&lt;k:
+                heapq.heappush(self.smallnums,-1*root.val)
+#            elif heapq.nsmallest(1,self.smallnums)[0]*-1 &gt; root.val:
+            elif self.smallnums[0]*-1 &gt; root.val:
+                heapq.heappop(self.smallnums)
+                heapq.heappush(self.smallnums,-1*root.val)
+            else:
+                pass
+                #do nothing
+            self.traverse(root.right, k)
+    def kthSmallest(self, root: Optional[TreeNode], k: int) -&gt; int:
+        self.traverse(root,k)
+        return self.smallnums[0]*-1</t>
+  </si>
+  <si>
+    <t>To find the kth smallest element in a binary search tree (BST), we leverage the property that an in-order traversal of a BST visits nodes in ascending order. We use a stack to help with this traversal:
+1. Start at the root and push all the left children onto the stack until there are no more left nodes.
+2. Pop the top node from the stack, which is the next smallest element in the BST.
+3. Decrease k by 1, as we've found the next smallest element.
+4. If k becomes 0, the current node's value is the kth smallest, so we return it.
+5. If not, move to the right child of the current node and repeat the process.
+By maintaining this in-order traversal using the stack, we efficiently find the kth smallest element without visiting all nodes, as we stop once we reach the desired element.
+FUNCTION kthSmallest(root, k)
+    INITIALIZE stack AS empty list
+    SET curr TO root
+    WHILE stack IS NOT empty OR curr IS NOT NULL
+        WHILE curr IS NOT NULL
+            ADD curr TO stack
+            SET curr TO curr.left
+        SET curr TO stack.pop()
+        DECREMENT k BY 1
+        IF k EQUALS 0
+            RETURN curr.val
+        SET curr TO curr.right
+END FUNCTION</t>
+  </si>
+  <si>
+    <t>travers left subtree to find kth smalles value. Otherwise find smallest and go right. Continue same process for its left subtree</t>
+  </si>
+  <si>
+    <t>Kth Smallest Element In a Bst </t>
+  </si>
+  <si>
+    <t>Validate Binary Search Tree </t>
   </si>
 </sst>
 </file>
@@ -1601,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D8D0A7-2B23-DB41-A123-92CA1A1D8EFD}">
   <dimension ref="A1:S216"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2431,12 +2515,45 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>152</v>
+      </c>
       <c r="F36" t="s">
         <v>13</v>
       </c>
+      <c r="G36" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>154</v>
+      </c>
       <c r="F37" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2863,6 +2980,8 @@
     <hyperlink ref="B33" r:id="rId32" display="https://neetcode.io/problems/subtree-of-a-binary-tree" xr:uid="{7B7A2977-FAAE-3E4D-9F52-976D1F4F4A17}"/>
     <hyperlink ref="B34" r:id="rId33" display="https://neetcode.io/problems/lowest-common-ancestor-in-binary-search-tree" xr:uid="{159CE993-32D5-5642-8C4D-75540899B343}"/>
     <hyperlink ref="B35" r:id="rId34" display="https://neetcode.io/problems/level-order-traversal-of-binary-tree" xr:uid="{C841EDDF-306D-8847-8EAE-F23A5F0494C7}"/>
+    <hyperlink ref="B37" r:id="rId35" display="https://neetcode.io/problems/kth-smallest-integer-in-bst" xr:uid="{2804BE54-CD1B-5847-BC91-01C1185BB0A7}"/>
+    <hyperlink ref="B36" r:id="rId36" display="https://neetcode.io/problems/valid-binary-search-tree" xr:uid="{03349B3C-ABAB-B94A-8A26-5E068E87E65A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
preorder inorder to tree construction of BST
</commit_message>
<xml_diff>
--- a/AlgoSheet/Algosheet.xlsx
+++ b/AlgoSheet/Algosheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhinavsivanandhan/Downloads/the-ab-repositories/DSA-Prep/AlgoSheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAAAAE0-FC4D-454C-AEE8-144BDA2CE4F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA9A243-FDF7-A644-9734-609E5466B3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27680" yWindow="2360" windowWidth="23360" windowHeight="14660" xr2:uid="{ABD715AC-0ABD-514F-973B-BA2370187A94}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="162">
   <si>
     <t>Category</t>
   </si>
@@ -1247,6 +1247,30 @@
   </si>
   <si>
     <t>Validate Binary Search Tree </t>
+  </si>
+  <si>
+    <t>Construct Binary Tree From Preorder And Inorder Traversal </t>
+  </si>
+  <si>
+    <t>use 2 facts. First value in preorder is always root, so construct that and give it its relevant part of preorder and inorder.
+Second is preorder and inorder consist of unique values. This is  a given contraint which is useful to implement</t>
+  </si>
+  <si>
+    <t># Definition for a binary tree node.
+# class TreeNode:
+#     def __init__(self, val=0, left=None, right=None):
+#         self.val = val
+#         self.left = left
+#         self.right = right
+class Solution:
+    def buildTree(self, preorder: List[int], inorder: List[int]) -&gt; Optional[TreeNode]:
+        if not preorder:#constraint given : Each value of inorder also appears in preorder. so we can just check one
+            return None
+        root = TreeNode(preorder[0])
+        mid = inorder.index(preorder[0])
+        root.left = self.buildTree(preorder[1:mid+1], inorder[:mid])
+        root.right = self.buildTree(preorder[mid+1:], inorder[mid+1:])
+        return root</t>
   </si>
 </sst>
 </file>
@@ -1686,7 +1710,7 @@
   <dimension ref="A1:S216"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36:G37"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2558,7 +2582,22 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>161</v>
+      </c>
       <c r="F38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2982,6 +3021,7 @@
     <hyperlink ref="B35" r:id="rId34" display="https://neetcode.io/problems/level-order-traversal-of-binary-tree" xr:uid="{C841EDDF-306D-8847-8EAE-F23A5F0494C7}"/>
     <hyperlink ref="B37" r:id="rId35" display="https://neetcode.io/problems/kth-smallest-integer-in-bst" xr:uid="{2804BE54-CD1B-5847-BC91-01C1185BB0A7}"/>
     <hyperlink ref="B36" r:id="rId36" display="https://neetcode.io/problems/valid-binary-search-tree" xr:uid="{03349B3C-ABAB-B94A-8A26-5E068E87E65A}"/>
+    <hyperlink ref="B38" r:id="rId37" display="https://neetcode.io/problems/binary-tree-from-preorder-and-inorder-traversal" xr:uid="{C00137CB-E00D-5E42-B4F5-2278B255197B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>